<commit_message>
add calculation of desired hospitalisation propensity to asympt excel
</commit_message>
<xml_diff>
--- a/data/interim/model_parameters/COVID19_SEIRD/wu_asymptomatic_fraction.xlsx
+++ b/data/interim/model_parameters/COVID19_SEIRD/wu_asymptomatic_fraction.xlsx
@@ -20,7 +20,10 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="23" uniqueCount="23">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="43" uniqueCount="30">
+  <si>
+    <t xml:space="preserve">age group</t>
+  </si>
   <si>
     <t xml:space="preserve">n0 individuals</t>
   </si>
@@ -89,6 +92,24 @@
   </si>
   <si>
     <t xml:space="preserve">So why was 43% symptomatic chosen? So that the symptomatic fraction in 80+ would equal 99%, this is in other words, an assumption I made.</t>
+  </si>
+  <si>
+    <t xml:space="preserve">fraction</t>
+  </si>
+  <si>
+    <t xml:space="preserve">fitted h</t>
+  </si>
+  <si>
+    <t xml:space="preserve">pop weighted h</t>
+  </si>
+  <si>
+    <t xml:space="preserve">desired h</t>
+  </si>
+  <si>
+    <t xml:space="preserve">rounded h (%)</t>
+  </si>
+  <si>
+    <t xml:space="preserve">desired pop weighted h</t>
   </si>
 </sst>
 </file>
@@ -191,7 +212,7 @@
     <xf numFmtId="42" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
     <xf numFmtId="9" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
   </cellStyleXfs>
-  <cellXfs count="8">
+  <cellXfs count="9">
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="false" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
@@ -221,6 +242,10 @@
       <protection locked="true" hidden="false"/>
     </xf>
     <xf numFmtId="164" fontId="6" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false">
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="165" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
@@ -301,47 +326,50 @@
   <sheetPr filterMode="false">
     <pageSetUpPr fitToPage="false"/>
   </sheetPr>
-  <dimension ref="A1:G21"/>
+  <dimension ref="A1:H38"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="I7" activeCellId="0" sqref="I7"/>
+      <selection pane="topLeft" activeCell="F19" activeCellId="0" sqref="F19"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
-    <col collapsed="false" customWidth="false" hidden="false" outlineLevel="0" max="1" min="1" style="0" width="11.52"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="0" width="20.01"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="0" width="12.9"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="3" min="3" style="0" width="17.21"/>
     <col collapsed="false" customWidth="false" hidden="false" outlineLevel="0" max="4" min="4" style="0" width="11.52"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="5" min="5" style="0" width="24.04"/>
-    <col collapsed="false" customWidth="false" hidden="false" outlineLevel="0" max="6" min="6" style="0" width="11.52"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="6" min="6" style="0" width="15.97"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="7" min="7" style="0" width="13.06"/>
     <col collapsed="false" customWidth="false" hidden="false" outlineLevel="0" max="1025" min="8" style="0" width="11.52"/>
   </cols>
   <sheetData>
     <row r="1" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A1" s="0" t="s">
+        <v>0</v>
+      </c>
       <c r="B1" s="0" t="s">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="C1" s="0" t="s">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="D1" s="0" t="s">
-        <v>2</v>
+        <v>3</v>
       </c>
       <c r="E1" s="0" t="s">
-        <v>3</v>
+        <v>4</v>
       </c>
       <c r="F1" s="1" t="s">
-        <v>4</v>
+        <v>5</v>
       </c>
       <c r="G1" s="2" t="s">
-        <v>5</v>
+        <v>6</v>
       </c>
     </row>
     <row r="2" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A2" s="0" t="s">
-        <v>6</v>
+        <v>7</v>
       </c>
       <c r="B2" s="0" t="n">
         <v>1305219</v>
@@ -366,7 +394,7 @@
     </row>
     <row r="3" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A3" s="0" t="s">
-        <v>7</v>
+        <v>8</v>
       </c>
       <c r="B3" s="0" t="n">
         <v>1298970</v>
@@ -389,7 +417,7 @@
     </row>
     <row r="4" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A4" s="0" t="s">
-        <v>8</v>
+        <v>9</v>
       </c>
       <c r="B4" s="0" t="n">
         <v>1395385</v>
@@ -412,7 +440,7 @@
     </row>
     <row r="5" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A5" s="0" t="s">
-        <v>9</v>
+        <v>10</v>
       </c>
       <c r="B5" s="0" t="n">
         <v>1498535</v>
@@ -435,7 +463,7 @@
     </row>
     <row r="6" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A6" s="0" t="s">
-        <v>10</v>
+        <v>11</v>
       </c>
       <c r="B6" s="0" t="n">
         <v>1524152</v>
@@ -458,7 +486,7 @@
     </row>
     <row r="7" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A7" s="0" t="s">
-        <v>11</v>
+        <v>12</v>
       </c>
       <c r="B7" s="0" t="n">
         <v>1601891</v>
@@ -481,7 +509,7 @@
     </row>
     <row r="8" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A8" s="0" t="s">
-        <v>12</v>
+        <v>13</v>
       </c>
       <c r="B8" s="0" t="n">
         <v>1347696</v>
@@ -504,7 +532,7 @@
     </row>
     <row r="9" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A9" s="0" t="s">
-        <v>13</v>
+        <v>14</v>
       </c>
       <c r="B9" s="0" t="n">
         <v>908725</v>
@@ -527,7 +555,7 @@
     </row>
     <row r="10" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A10" s="0" t="s">
-        <v>14</v>
+        <v>15</v>
       </c>
       <c r="B10" s="0" t="n">
         <v>658753</v>
@@ -550,7 +578,7 @@
     </row>
     <row r="11" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A11" s="0" t="s">
-        <v>15</v>
+        <v>16</v>
       </c>
       <c r="B11" s="0" t="n">
         <f aca="false">SUM(B2:B10)</f>
@@ -567,7 +595,7 @@
     </row>
     <row r="13" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A13" s="0" t="s">
-        <v>16</v>
+        <v>17</v>
       </c>
       <c r="B13" s="0" t="n">
         <v>0.43</v>
@@ -581,32 +609,329 @@
     </row>
     <row r="16" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A16" s="6" t="s">
-        <v>17</v>
+        <v>18</v>
       </c>
     </row>
     <row r="17" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A17" s="7" t="s">
-        <v>18</v>
+        <v>19</v>
       </c>
     </row>
     <row r="18" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A18" s="0" t="s">
-        <v>19</v>
+        <v>20</v>
       </c>
     </row>
     <row r="19" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A19" s="0" t="s">
-        <v>20</v>
+        <v>21</v>
       </c>
     </row>
     <row r="20" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A20" s="0" t="s">
-        <v>21</v>
+        <v>22</v>
       </c>
     </row>
     <row r="21" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A21" s="0" t="s">
-        <v>22</v>
+        <v>23</v>
+      </c>
+    </row>
+    <row r="25" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A25" s="0" t="s">
+        <v>0</v>
+      </c>
+      <c r="B25" s="0" t="s">
+        <v>1</v>
+      </c>
+      <c r="C25" s="0" t="s">
+        <v>24</v>
+      </c>
+      <c r="D25" s="0" t="s">
+        <v>25</v>
+      </c>
+      <c r="E25" s="0" t="s">
+        <v>3</v>
+      </c>
+      <c r="F25" s="0" t="s">
+        <v>26</v>
+      </c>
+      <c r="G25" s="0" t="s">
+        <v>27</v>
+      </c>
+      <c r="H25" s="0" t="s">
+        <v>28</v>
+      </c>
+    </row>
+    <row r="26" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A26" s="0" t="s">
+        <v>7</v>
+      </c>
+      <c r="B26" s="0" t="n">
+        <v>1305219</v>
+      </c>
+      <c r="C26" s="0" t="n">
+        <f aca="false">B26/$B$35</f>
+        <v>0.113110505760908</v>
+      </c>
+      <c r="D26" s="0" t="n">
+        <v>0.015</v>
+      </c>
+      <c r="E26" s="0" t="n">
+        <v>0.746784953353961</v>
+      </c>
+      <c r="F26" s="0" t="n">
+        <f aca="false">D26*$E$26*C26</f>
+        <v>0.00126703835652754</v>
+      </c>
+      <c r="G26" s="0" t="n">
+        <f aca="false">D26*$E$26</f>
+        <v>0.0112017743003094</v>
+      </c>
+      <c r="H26" s="0" t="n">
+        <f aca="false">ROUND(G26,3)*100</f>
+        <v>1.1</v>
+      </c>
+    </row>
+    <row r="27" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A27" s="0" t="s">
+        <v>8</v>
+      </c>
+      <c r="B27" s="0" t="n">
+        <v>1298970</v>
+      </c>
+      <c r="C27" s="0" t="n">
+        <f aca="false">B27/$B$35</f>
+        <v>0.112568966333042</v>
+      </c>
+      <c r="D27" s="0" t="n">
+        <v>0.02</v>
+      </c>
+      <c r="F27" s="0" t="n">
+        <f aca="false">D27*$E$26*C27</f>
+        <v>0.00168129620544249</v>
+      </c>
+      <c r="G27" s="0" t="n">
+        <f aca="false">D27*$E$26</f>
+        <v>0.0149356990670792</v>
+      </c>
+      <c r="H27" s="0" t="n">
+        <f aca="false">ROUND(G27,3)*100</f>
+        <v>1.5</v>
+      </c>
+    </row>
+    <row r="28" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A28" s="0" t="s">
+        <v>9</v>
+      </c>
+      <c r="B28" s="0" t="n">
+        <v>1395385</v>
+      </c>
+      <c r="C28" s="0" t="n">
+        <f aca="false">B28/$B$35</f>
+        <v>0.120924307017585</v>
+      </c>
+      <c r="D28" s="0" t="n">
+        <v>0.03</v>
+      </c>
+      <c r="F28" s="0" t="n">
+        <f aca="false">D28*$E$26*C28</f>
+        <v>0.00270913358926462</v>
+      </c>
+      <c r="G28" s="0" t="n">
+        <f aca="false">D28*$E$26</f>
+        <v>0.0224035486006188</v>
+      </c>
+      <c r="H28" s="0" t="n">
+        <f aca="false">ROUND(G28,3)*100</f>
+        <v>2.2</v>
+      </c>
+    </row>
+    <row r="29" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A29" s="0" t="s">
+        <v>10</v>
+      </c>
+      <c r="B29" s="0" t="n">
+        <v>1498535</v>
+      </c>
+      <c r="C29" s="0" t="n">
+        <f aca="false">B29/$B$35</f>
+        <v>0.1298633039746</v>
+      </c>
+      <c r="D29" s="0" t="n">
+        <v>0.03</v>
+      </c>
+      <c r="F29" s="0" t="n">
+        <f aca="false">D29*$E$26*C29</f>
+        <v>0.00290939884203188</v>
+      </c>
+      <c r="G29" s="0" t="n">
+        <f aca="false">D29*$E$26</f>
+        <v>0.0224035486006188</v>
+      </c>
+      <c r="H29" s="0" t="n">
+        <f aca="false">ROUND(G29,3)*100</f>
+        <v>2.2</v>
+      </c>
+    </row>
+    <row r="30" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A30" s="0" t="s">
+        <v>11</v>
+      </c>
+      <c r="B30" s="0" t="n">
+        <v>1524152</v>
+      </c>
+      <c r="C30" s="0" t="n">
+        <f aca="false">B30/$B$35</f>
+        <v>0.132083277654172</v>
+      </c>
+      <c r="D30" s="0" t="n">
+        <v>0.03</v>
+      </c>
+      <c r="F30" s="0" t="n">
+        <f aca="false">D30*$E$26*C30</f>
+        <v>0.00295913413025426</v>
+      </c>
+      <c r="G30" s="0" t="n">
+        <f aca="false">D30*$E$26</f>
+        <v>0.0224035486006188</v>
+      </c>
+      <c r="H30" s="0" t="n">
+        <f aca="false">ROUND(G30,3)*100</f>
+        <v>2.2</v>
+      </c>
+    </row>
+    <row r="31" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A31" s="0" t="s">
+        <v>12</v>
+      </c>
+      <c r="B31" s="0" t="n">
+        <v>1601891</v>
+      </c>
+      <c r="C31" s="0" t="n">
+        <f aca="false">B31/$B$35</f>
+        <v>0.138820152927476</v>
+      </c>
+      <c r="D31" s="0" t="n">
+        <v>0.06</v>
+      </c>
+      <c r="F31" s="0" t="n">
+        <f aca="false">D31*$E$26*C31</f>
+        <v>0.00622012808571209</v>
+      </c>
+      <c r="G31" s="0" t="n">
+        <f aca="false">D31*$E$26</f>
+        <v>0.0448070972012377</v>
+      </c>
+      <c r="H31" s="0" t="n">
+        <f aca="false">ROUND(G31,3)*100</f>
+        <v>4.5</v>
+      </c>
+    </row>
+    <row r="32" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A32" s="0" t="s">
+        <v>13</v>
+      </c>
+      <c r="B32" s="0" t="n">
+        <v>1347696</v>
+      </c>
+      <c r="C32" s="0" t="n">
+        <f aca="false">B32/$B$35</f>
+        <v>0.116791569975577</v>
+      </c>
+      <c r="D32" s="0" t="n">
+        <v>0.14</v>
+      </c>
+      <c r="F32" s="0" t="n">
+        <f aca="false">D32*$E$26*C32</f>
+        <v>0.0122105461990887</v>
+      </c>
+      <c r="G32" s="0" t="n">
+        <f aca="false">D32*$E$26</f>
+        <v>0.104549893469555</v>
+      </c>
+      <c r="H32" s="0" t="n">
+        <f aca="false">ROUND(G32,3)*100</f>
+        <v>10.5</v>
+      </c>
+    </row>
+    <row r="33" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A33" s="0" t="s">
+        <v>14</v>
+      </c>
+      <c r="B33" s="0" t="n">
+        <v>908725</v>
+      </c>
+      <c r="C33" s="0" t="n">
+        <f aca="false">B33/$B$35</f>
+        <v>0.0787502666966858</v>
+      </c>
+      <c r="D33" s="0" t="n">
+        <v>0.3</v>
+      </c>
+      <c r="F33" s="0" t="n">
+        <f aca="false">D33*$E$26*C33</f>
+        <v>0.0176428542725089</v>
+      </c>
+      <c r="G33" s="0" t="n">
+        <f aca="false">D33*$E$26</f>
+        <v>0.224035486006188</v>
+      </c>
+      <c r="H33" s="0" t="n">
+        <f aca="false">ROUND(G33,3)*100</f>
+        <v>22.4</v>
+      </c>
+    </row>
+    <row r="34" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A34" s="0" t="s">
+        <v>15</v>
+      </c>
+      <c r="B34" s="0" t="n">
+        <v>658753</v>
+      </c>
+      <c r="C34" s="0" t="n">
+        <f aca="false">B34/$B$35</f>
+        <v>0.0570876496599542</v>
+      </c>
+      <c r="D34" s="0" t="n">
+        <v>0.76</v>
+      </c>
+      <c r="F34" s="0" t="n">
+        <f aca="false">D34*$E$26*C34</f>
+        <v>0.0324004703191811</v>
+      </c>
+      <c r="G34" s="0" t="n">
+        <f aca="false">D34*$E$26</f>
+        <v>0.567556564549011</v>
+      </c>
+      <c r="H34" s="0" t="n">
+        <f aca="false">ROUND(G34,3)*100</f>
+        <v>56.8</v>
+      </c>
+    </row>
+    <row r="35" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A35" s="0" t="s">
+        <v>16</v>
+      </c>
+      <c r="B35" s="0" t="n">
+        <f aca="false">SUM(B26:B34)</f>
+        <v>11539326</v>
+      </c>
+      <c r="C35" s="0" t="n">
+        <f aca="false">B35/$B$35</f>
+        <v>1</v>
+      </c>
+      <c r="F35" s="8" t="n">
+        <f aca="false">SUM(F26:F34)</f>
+        <v>0.0800000000000115</v>
+      </c>
+    </row>
+    <row r="38" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A38" s="0" t="s">
+        <v>29</v>
+      </c>
+      <c r="B38" s="8" t="n">
+        <v>0.08</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Manuscript R2 - data analysis hospitals (#278)
</commit_message>
<xml_diff>
--- a/data/interim/model_parameters/COVID19_SEIRD/wu_asymptomatic_fraction.xlsx
+++ b/data/interim/model_parameters/COVID19_SEIRD/wu_asymptomatic_fraction.xlsx
@@ -20,7 +20,10 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="23" uniqueCount="23">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="43" uniqueCount="30">
+  <si>
+    <t xml:space="preserve">age group</t>
+  </si>
   <si>
     <t xml:space="preserve">n0 individuals</t>
   </si>
@@ -89,6 +92,24 @@
   </si>
   <si>
     <t xml:space="preserve">So why was 43% symptomatic chosen? So that the symptomatic fraction in 80+ would equal 99%, this is in other words, an assumption I made.</t>
+  </si>
+  <si>
+    <t xml:space="preserve">fraction</t>
+  </si>
+  <si>
+    <t xml:space="preserve">fitted h</t>
+  </si>
+  <si>
+    <t xml:space="preserve">pop weighted h</t>
+  </si>
+  <si>
+    <t xml:space="preserve">desired h</t>
+  </si>
+  <si>
+    <t xml:space="preserve">rounded h (%)</t>
+  </si>
+  <si>
+    <t xml:space="preserve">desired pop weighted h</t>
   </si>
 </sst>
 </file>
@@ -191,7 +212,7 @@
     <xf numFmtId="42" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
     <xf numFmtId="9" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
   </cellStyleXfs>
-  <cellXfs count="8">
+  <cellXfs count="9">
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="false" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
@@ -221,6 +242,10 @@
       <protection locked="true" hidden="false"/>
     </xf>
     <xf numFmtId="164" fontId="6" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false">
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="165" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
@@ -301,47 +326,50 @@
   <sheetPr filterMode="false">
     <pageSetUpPr fitToPage="false"/>
   </sheetPr>
-  <dimension ref="A1:G21"/>
+  <dimension ref="A1:H38"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="I7" activeCellId="0" sqref="I7"/>
+      <selection pane="topLeft" activeCell="F19" activeCellId="0" sqref="F19"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
-    <col collapsed="false" customWidth="false" hidden="false" outlineLevel="0" max="1" min="1" style="0" width="11.52"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="0" width="20.01"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="0" width="12.9"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="3" min="3" style="0" width="17.21"/>
     <col collapsed="false" customWidth="false" hidden="false" outlineLevel="0" max="4" min="4" style="0" width="11.52"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="5" min="5" style="0" width="24.04"/>
-    <col collapsed="false" customWidth="false" hidden="false" outlineLevel="0" max="6" min="6" style="0" width="11.52"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="6" min="6" style="0" width="15.97"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="7" min="7" style="0" width="13.06"/>
     <col collapsed="false" customWidth="false" hidden="false" outlineLevel="0" max="1025" min="8" style="0" width="11.52"/>
   </cols>
   <sheetData>
     <row r="1" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A1" s="0" t="s">
+        <v>0</v>
+      </c>
       <c r="B1" s="0" t="s">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="C1" s="0" t="s">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="D1" s="0" t="s">
-        <v>2</v>
+        <v>3</v>
       </c>
       <c r="E1" s="0" t="s">
-        <v>3</v>
+        <v>4</v>
       </c>
       <c r="F1" s="1" t="s">
-        <v>4</v>
+        <v>5</v>
       </c>
       <c r="G1" s="2" t="s">
-        <v>5</v>
+        <v>6</v>
       </c>
     </row>
     <row r="2" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A2" s="0" t="s">
-        <v>6</v>
+        <v>7</v>
       </c>
       <c r="B2" s="0" t="n">
         <v>1305219</v>
@@ -366,7 +394,7 @@
     </row>
     <row r="3" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A3" s="0" t="s">
-        <v>7</v>
+        <v>8</v>
       </c>
       <c r="B3" s="0" t="n">
         <v>1298970</v>
@@ -389,7 +417,7 @@
     </row>
     <row r="4" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A4" s="0" t="s">
-        <v>8</v>
+        <v>9</v>
       </c>
       <c r="B4" s="0" t="n">
         <v>1395385</v>
@@ -412,7 +440,7 @@
     </row>
     <row r="5" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A5" s="0" t="s">
-        <v>9</v>
+        <v>10</v>
       </c>
       <c r="B5" s="0" t="n">
         <v>1498535</v>
@@ -435,7 +463,7 @@
     </row>
     <row r="6" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A6" s="0" t="s">
-        <v>10</v>
+        <v>11</v>
       </c>
       <c r="B6" s="0" t="n">
         <v>1524152</v>
@@ -458,7 +486,7 @@
     </row>
     <row r="7" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A7" s="0" t="s">
-        <v>11</v>
+        <v>12</v>
       </c>
       <c r="B7" s="0" t="n">
         <v>1601891</v>
@@ -481,7 +509,7 @@
     </row>
     <row r="8" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A8" s="0" t="s">
-        <v>12</v>
+        <v>13</v>
       </c>
       <c r="B8" s="0" t="n">
         <v>1347696</v>
@@ -504,7 +532,7 @@
     </row>
     <row r="9" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A9" s="0" t="s">
-        <v>13</v>
+        <v>14</v>
       </c>
       <c r="B9" s="0" t="n">
         <v>908725</v>
@@ -527,7 +555,7 @@
     </row>
     <row r="10" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A10" s="0" t="s">
-        <v>14</v>
+        <v>15</v>
       </c>
       <c r="B10" s="0" t="n">
         <v>658753</v>
@@ -550,7 +578,7 @@
     </row>
     <row r="11" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A11" s="0" t="s">
-        <v>15</v>
+        <v>16</v>
       </c>
       <c r="B11" s="0" t="n">
         <f aca="false">SUM(B2:B10)</f>
@@ -567,7 +595,7 @@
     </row>
     <row r="13" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A13" s="0" t="s">
-        <v>16</v>
+        <v>17</v>
       </c>
       <c r="B13" s="0" t="n">
         <v>0.43</v>
@@ -581,32 +609,329 @@
     </row>
     <row r="16" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A16" s="6" t="s">
-        <v>17</v>
+        <v>18</v>
       </c>
     </row>
     <row r="17" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A17" s="7" t="s">
-        <v>18</v>
+        <v>19</v>
       </c>
     </row>
     <row r="18" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A18" s="0" t="s">
-        <v>19</v>
+        <v>20</v>
       </c>
     </row>
     <row r="19" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A19" s="0" t="s">
-        <v>20</v>
+        <v>21</v>
       </c>
     </row>
     <row r="20" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A20" s="0" t="s">
-        <v>21</v>
+        <v>22</v>
       </c>
     </row>
     <row r="21" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A21" s="0" t="s">
-        <v>22</v>
+        <v>23</v>
+      </c>
+    </row>
+    <row r="25" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A25" s="0" t="s">
+        <v>0</v>
+      </c>
+      <c r="B25" s="0" t="s">
+        <v>1</v>
+      </c>
+      <c r="C25" s="0" t="s">
+        <v>24</v>
+      </c>
+      <c r="D25" s="0" t="s">
+        <v>25</v>
+      </c>
+      <c r="E25" s="0" t="s">
+        <v>3</v>
+      </c>
+      <c r="F25" s="0" t="s">
+        <v>26</v>
+      </c>
+      <c r="G25" s="0" t="s">
+        <v>27</v>
+      </c>
+      <c r="H25" s="0" t="s">
+        <v>28</v>
+      </c>
+    </row>
+    <row r="26" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A26" s="0" t="s">
+        <v>7</v>
+      </c>
+      <c r="B26" s="0" t="n">
+        <v>1305219</v>
+      </c>
+      <c r="C26" s="0" t="n">
+        <f aca="false">B26/$B$35</f>
+        <v>0.113110505760908</v>
+      </c>
+      <c r="D26" s="0" t="n">
+        <v>0.015</v>
+      </c>
+      <c r="E26" s="0" t="n">
+        <v>0.746784953353961</v>
+      </c>
+      <c r="F26" s="0" t="n">
+        <f aca="false">D26*$E$26*C26</f>
+        <v>0.00126703835652754</v>
+      </c>
+      <c r="G26" s="0" t="n">
+        <f aca="false">D26*$E$26</f>
+        <v>0.0112017743003094</v>
+      </c>
+      <c r="H26" s="0" t="n">
+        <f aca="false">ROUND(G26,3)*100</f>
+        <v>1.1</v>
+      </c>
+    </row>
+    <row r="27" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A27" s="0" t="s">
+        <v>8</v>
+      </c>
+      <c r="B27" s="0" t="n">
+        <v>1298970</v>
+      </c>
+      <c r="C27" s="0" t="n">
+        <f aca="false">B27/$B$35</f>
+        <v>0.112568966333042</v>
+      </c>
+      <c r="D27" s="0" t="n">
+        <v>0.02</v>
+      </c>
+      <c r="F27" s="0" t="n">
+        <f aca="false">D27*$E$26*C27</f>
+        <v>0.00168129620544249</v>
+      </c>
+      <c r="G27" s="0" t="n">
+        <f aca="false">D27*$E$26</f>
+        <v>0.0149356990670792</v>
+      </c>
+      <c r="H27" s="0" t="n">
+        <f aca="false">ROUND(G27,3)*100</f>
+        <v>1.5</v>
+      </c>
+    </row>
+    <row r="28" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A28" s="0" t="s">
+        <v>9</v>
+      </c>
+      <c r="B28" s="0" t="n">
+        <v>1395385</v>
+      </c>
+      <c r="C28" s="0" t="n">
+        <f aca="false">B28/$B$35</f>
+        <v>0.120924307017585</v>
+      </c>
+      <c r="D28" s="0" t="n">
+        <v>0.03</v>
+      </c>
+      <c r="F28" s="0" t="n">
+        <f aca="false">D28*$E$26*C28</f>
+        <v>0.00270913358926462</v>
+      </c>
+      <c r="G28" s="0" t="n">
+        <f aca="false">D28*$E$26</f>
+        <v>0.0224035486006188</v>
+      </c>
+      <c r="H28" s="0" t="n">
+        <f aca="false">ROUND(G28,3)*100</f>
+        <v>2.2</v>
+      </c>
+    </row>
+    <row r="29" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A29" s="0" t="s">
+        <v>10</v>
+      </c>
+      <c r="B29" s="0" t="n">
+        <v>1498535</v>
+      </c>
+      <c r="C29" s="0" t="n">
+        <f aca="false">B29/$B$35</f>
+        <v>0.1298633039746</v>
+      </c>
+      <c r="D29" s="0" t="n">
+        <v>0.03</v>
+      </c>
+      <c r="F29" s="0" t="n">
+        <f aca="false">D29*$E$26*C29</f>
+        <v>0.00290939884203188</v>
+      </c>
+      <c r="G29" s="0" t="n">
+        <f aca="false">D29*$E$26</f>
+        <v>0.0224035486006188</v>
+      </c>
+      <c r="H29" s="0" t="n">
+        <f aca="false">ROUND(G29,3)*100</f>
+        <v>2.2</v>
+      </c>
+    </row>
+    <row r="30" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A30" s="0" t="s">
+        <v>11</v>
+      </c>
+      <c r="B30" s="0" t="n">
+        <v>1524152</v>
+      </c>
+      <c r="C30" s="0" t="n">
+        <f aca="false">B30/$B$35</f>
+        <v>0.132083277654172</v>
+      </c>
+      <c r="D30" s="0" t="n">
+        <v>0.03</v>
+      </c>
+      <c r="F30" s="0" t="n">
+        <f aca="false">D30*$E$26*C30</f>
+        <v>0.00295913413025426</v>
+      </c>
+      <c r="G30" s="0" t="n">
+        <f aca="false">D30*$E$26</f>
+        <v>0.0224035486006188</v>
+      </c>
+      <c r="H30" s="0" t="n">
+        <f aca="false">ROUND(G30,3)*100</f>
+        <v>2.2</v>
+      </c>
+    </row>
+    <row r="31" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A31" s="0" t="s">
+        <v>12</v>
+      </c>
+      <c r="B31" s="0" t="n">
+        <v>1601891</v>
+      </c>
+      <c r="C31" s="0" t="n">
+        <f aca="false">B31/$B$35</f>
+        <v>0.138820152927476</v>
+      </c>
+      <c r="D31" s="0" t="n">
+        <v>0.06</v>
+      </c>
+      <c r="F31" s="0" t="n">
+        <f aca="false">D31*$E$26*C31</f>
+        <v>0.00622012808571209</v>
+      </c>
+      <c r="G31" s="0" t="n">
+        <f aca="false">D31*$E$26</f>
+        <v>0.0448070972012377</v>
+      </c>
+      <c r="H31" s="0" t="n">
+        <f aca="false">ROUND(G31,3)*100</f>
+        <v>4.5</v>
+      </c>
+    </row>
+    <row r="32" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A32" s="0" t="s">
+        <v>13</v>
+      </c>
+      <c r="B32" s="0" t="n">
+        <v>1347696</v>
+      </c>
+      <c r="C32" s="0" t="n">
+        <f aca="false">B32/$B$35</f>
+        <v>0.116791569975577</v>
+      </c>
+      <c r="D32" s="0" t="n">
+        <v>0.14</v>
+      </c>
+      <c r="F32" s="0" t="n">
+        <f aca="false">D32*$E$26*C32</f>
+        <v>0.0122105461990887</v>
+      </c>
+      <c r="G32" s="0" t="n">
+        <f aca="false">D32*$E$26</f>
+        <v>0.104549893469555</v>
+      </c>
+      <c r="H32" s="0" t="n">
+        <f aca="false">ROUND(G32,3)*100</f>
+        <v>10.5</v>
+      </c>
+    </row>
+    <row r="33" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A33" s="0" t="s">
+        <v>14</v>
+      </c>
+      <c r="B33" s="0" t="n">
+        <v>908725</v>
+      </c>
+      <c r="C33" s="0" t="n">
+        <f aca="false">B33/$B$35</f>
+        <v>0.0787502666966858</v>
+      </c>
+      <c r="D33" s="0" t="n">
+        <v>0.3</v>
+      </c>
+      <c r="F33" s="0" t="n">
+        <f aca="false">D33*$E$26*C33</f>
+        <v>0.0176428542725089</v>
+      </c>
+      <c r="G33" s="0" t="n">
+        <f aca="false">D33*$E$26</f>
+        <v>0.224035486006188</v>
+      </c>
+      <c r="H33" s="0" t="n">
+        <f aca="false">ROUND(G33,3)*100</f>
+        <v>22.4</v>
+      </c>
+    </row>
+    <row r="34" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A34" s="0" t="s">
+        <v>15</v>
+      </c>
+      <c r="B34" s="0" t="n">
+        <v>658753</v>
+      </c>
+      <c r="C34" s="0" t="n">
+        <f aca="false">B34/$B$35</f>
+        <v>0.0570876496599542</v>
+      </c>
+      <c r="D34" s="0" t="n">
+        <v>0.76</v>
+      </c>
+      <c r="F34" s="0" t="n">
+        <f aca="false">D34*$E$26*C34</f>
+        <v>0.0324004703191811</v>
+      </c>
+      <c r="G34" s="0" t="n">
+        <f aca="false">D34*$E$26</f>
+        <v>0.567556564549011</v>
+      </c>
+      <c r="H34" s="0" t="n">
+        <f aca="false">ROUND(G34,3)*100</f>
+        <v>56.8</v>
+      </c>
+    </row>
+    <row r="35" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A35" s="0" t="s">
+        <v>16</v>
+      </c>
+      <c r="B35" s="0" t="n">
+        <f aca="false">SUM(B26:B34)</f>
+        <v>11539326</v>
+      </c>
+      <c r="C35" s="0" t="n">
+        <f aca="false">B35/$B$35</f>
+        <v>1</v>
+      </c>
+      <c r="F35" s="8" t="n">
+        <f aca="false">SUM(F26:F34)</f>
+        <v>0.0800000000000115</v>
+      </c>
+    </row>
+    <row r="38" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A38" s="0" t="s">
+        <v>29</v>
+      </c>
+      <c r="B38" s="8" t="n">
+        <v>0.08</v>
       </c>
     </row>
   </sheetData>

</xml_diff>